<commit_message>
Validating EVE component (Amdo)
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-amdo-refseqs-side-data.xlsx
+++ b/tabular/eve/epv-amdo-refseqs-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A7F442-E512-AE40-A2E9-B39567FA631B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6846B0D4-3DB0-994B-8957-C8717EC4A687}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="6440" windowWidth="32880" windowHeight="17240" xr2:uid="{7DFEF833-9CB6-184F-AD64-EB162905208A}"/>
+    <workbookView xWindow="9040" yWindow="9680" windowWidth="32880" windowHeight="17240" xr2:uid="{7DFEF833-9CB6-184F-AD64-EB162905208A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -107,18 +107,6 @@
     <t>amdo.2-ellobius</t>
   </si>
   <si>
-    <t>amdo.101-protobothrops</t>
-  </si>
-  <si>
-    <t>amdo.102-procavia</t>
-  </si>
-  <si>
-    <t>amdo.103-orycteropus</t>
-  </si>
-  <si>
-    <t>amdo.104-sarcophilus</t>
-  </si>
-  <si>
     <t>fasta-refseqs-amdo-epv</t>
   </si>
   <si>
@@ -144,6 +132,18 @@
   </si>
   <si>
     <t>assign_subclade</t>
+  </si>
+  <si>
+    <t>ap.102-procavia</t>
+  </si>
+  <si>
+    <t>ap.103-orycteropus</t>
+  </si>
+  <si>
+    <t>ap.104-sarcophilus</t>
+  </si>
+  <si>
+    <t>ap.101-serpentes-UR</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05DEEDB-7439-774B-BFFC-655641BD9B32}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B12:C13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
@@ -628,10 +628,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>5</v>
@@ -681,7 +681,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>22</v>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>21</v>
@@ -717,33 +717,33 @@
         <v>22</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="U2" s="10">
         <v>30443409</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -752,7 +752,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>22</v>
@@ -761,7 +761,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>21</v>
@@ -788,42 +788,42 @@
         <v>22</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O3" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U3" s="10">
         <v>30443409</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>22</v>
@@ -832,7 +832,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>21</v>
@@ -859,42 +859,42 @@
         <v>22</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U4" s="10">
         <v>30443409</v>
       </c>
-      <c r="V4" t="s">
-        <v>24</v>
-      </c>
-      <c r="W4" t="s">
-        <v>24</v>
+      <c r="V4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>22</v>
@@ -903,7 +903,7 @@
         <v>102</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>21</v>
@@ -930,42 +930,42 @@
         <v>22</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O5" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U5" s="10">
         <v>30443409</v>
       </c>
-      <c r="V5" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" t="s">
-        <v>25</v>
+      <c r="V5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>22</v>
@@ -974,7 +974,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>21</v>
@@ -1001,42 +1001,42 @@
         <v>22</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O6" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T6" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U6" s="10">
         <v>30443409</v>
       </c>
-      <c r="V6" t="s">
-        <v>26</v>
-      </c>
-      <c r="W6" t="s">
-        <v>26</v>
+      <c r="V6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>22</v>
@@ -1045,7 +1045,7 @@
         <v>104</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>21</v>
@@ -1072,34 +1072,34 @@
         <v>22</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O7" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="U7" s="10">
         <v>30443409</v>
       </c>
-      <c r="V7" t="s">
-        <v>27</v>
-      </c>
-      <c r="W7" t="s">
-        <v>27</v>
+      <c r="V7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>